<commit_message>
Update: M_2016 not required
</commit_message>
<xml_diff>
--- a/nscod16-step1.xlsx
+++ b/nscod16-step1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\x\dtu\steps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\dtu\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2627,27 +2627,12 @@
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
-      <c r="R45">
-        <v>2016</v>
-      </c>
-      <c r="S45" s="8">
-        <v>1.3260000000000001</v>
-      </c>
-      <c r="T45" s="8">
-        <v>0.96199999999999997</v>
-      </c>
-      <c r="U45" s="8">
-        <v>0.23300000000000001</v>
-      </c>
-      <c r="V45" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="W45" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="X45" s="8">
-        <v>0.2</v>
-      </c>
+      <c r="S45" s="8"/>
+      <c r="T45" s="8"/>
+      <c r="U45" s="8"/>
+      <c r="V45" s="8"/>
+      <c r="W45" s="8"/>
+      <c r="X45" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>